<commit_message>
Stage before using layouts. Fixed absolute positions are no longer the target.
</commit_message>
<xml_diff>
--- a/Munchkin.xlsx
+++ b/Munchkin.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="361">
   <si>
     <t>Создан 28.02</t>
   </si>
@@ -1079,6 +1079,36 @@
   </si>
   <si>
     <t>http://stackoverflow.com/questions/8693569/how-to-create-circle-icon-from-image-file</t>
+  </si>
+  <si>
+    <t>https://www.opennet.ru/docs/RUS/qt3_prog/c3346.html</t>
+  </si>
+  <si>
+    <t>По порядку:</t>
+  </si>
+  <si>
+    <t>1) Определиться с составом класса "Игрок"</t>
+  </si>
+  <si>
+    <t>Черновым образом</t>
+  </si>
+  <si>
+    <t>2) Расставить игроков и их кнопки на мониторе</t>
+  </si>
+  <si>
+    <t>По сути - определить размеры всех виджетов в долях от процентов экрана</t>
+  </si>
+  <si>
+    <t>Сделать размеры всех основных виджетов зависимыми от размеров кнопки "Аватар"</t>
+  </si>
+  <si>
+    <t>Т.о. при изменении этого единственного размера все будут пересчитываться</t>
+  </si>
+  <si>
+    <t>3) Написать алгоритм созлания игроков</t>
+  </si>
+  <si>
+    <t>Реализовать его в виде функции, вызываемой Игрой</t>
   </si>
 </sst>
 </file>
@@ -1114,12 +1144,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1135,7 +1171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1150,6 +1186,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1467,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H53"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1700,6 +1739,52 @@
         <v>350</v>
       </c>
     </row>
+    <row r="56" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>42890</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B60" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="D60" s="2">
+        <v>42890</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C19" r:id="rId1"/>
@@ -1713,9 +1798,10 @@
     <hyperlink ref="B43" r:id="rId9"/>
     <hyperlink ref="D51" r:id="rId10"/>
     <hyperlink ref="C53" r:id="rId11"/>
+    <hyperlink ref="B56" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId13"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Signals/slots functionality has been added to the Server
</commit_message>
<xml_diff>
--- a/Munchkin.xlsx
+++ b/Munchkin.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="370">
   <si>
     <t>Создан 28.02</t>
   </si>
@@ -1109,6 +1109,33 @@
   </si>
   <si>
     <t>Реализовать его в виде функции, вызываемой Игрой</t>
+  </si>
+  <si>
+    <t>Бранчевать</t>
+  </si>
+  <si>
+    <t>С целью выделять фичи</t>
+  </si>
+  <si>
+    <t>Написать алгоритм игры</t>
+  </si>
+  <si>
+    <t>Ответы сервера сделать загулшками</t>
+  </si>
+  <si>
+    <t>QtLogger</t>
+  </si>
+  <si>
+    <t>CuteLogger</t>
+  </si>
+  <si>
+    <t>std::vector&lt;GamerWidget*&gt;</t>
+  </si>
+  <si>
+    <t>Чтобы динамически добавлять</t>
+  </si>
+  <si>
+    <t>constexpr size_t maxOponentCount = 6;</t>
   </si>
 </sst>
 </file>
@@ -1185,10 +1212,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1506,16 +1533,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="16.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" style="1" customWidth="1"/>
@@ -1753,10 +1780,10 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="5" t="s">
         <v>354</v>
       </c>
       <c r="D60" s="2">
@@ -1783,6 +1810,46 @@
       </c>
       <c r="C62" s="1" t="s">
         <v>360</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>42921</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -2079,42 +2146,42 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -2430,42 +2497,42 @@
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
     </row>
     <row r="38" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
@@ -2793,42 +2860,42 @@
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="5"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="5"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
     </row>
     <row r="59" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
@@ -2977,42 +3044,42 @@
       </c>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
-      <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
-      <c r="J68" s="5"/>
-      <c r="K68" s="5"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
     </row>
     <row r="70" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
@@ -3429,42 +3496,42 @@
       </c>
     </row>
     <row r="103" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="C103" s="5"/>
-      <c r="D103" s="5"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="5"/>
-      <c r="G103" s="5"/>
-      <c r="H103" s="5"/>
-      <c r="I103" s="5"/>
-      <c r="J103" s="5"/>
-      <c r="K103" s="5"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="6"/>
+      <c r="K103" s="6"/>
     </row>
     <row r="104" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B104" s="5"/>
-      <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5"/>
-      <c r="H104" s="5"/>
-      <c r="I104" s="5"/>
-      <c r="J104" s="5"/>
-      <c r="K104" s="5"/>
+      <c r="B104" s="6"/>
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="6"/>
+      <c r="J104" s="6"/>
+      <c r="K104" s="6"/>
     </row>
     <row r="105" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B105" s="5"/>
-      <c r="C105" s="5"/>
-      <c r="D105" s="5"/>
-      <c r="E105" s="5"/>
-      <c r="F105" s="5"/>
-      <c r="G105" s="5"/>
-      <c r="H105" s="5"/>
-      <c r="I105" s="5"/>
-      <c r="J105" s="5"/>
-      <c r="K105" s="5"/>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="6"/>
+      <c r="K105" s="6"/>
     </row>
     <row r="107" spans="2:11" ht="135" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="s">

</xml_diff>